<commit_message>
fix to column ordering
</commit_message>
<xml_diff>
--- a/workbooks/output.xlsx
+++ b/workbooks/output.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="49">
   <si>
     <t>last_name</t>
   </si>
@@ -56,7 +56,13 @@
     <t>EC</t>
   </si>
   <si>
-    <t>2019-01-01</t>
+    <t>2018-01-01</t>
+  </si>
+  <si>
+    <t>2018-06-21</t>
+  </si>
+  <si>
+    <t>2018-06-22</t>
   </si>
   <si>
     <t>2019-06-21</t>
@@ -65,7 +71,13 @@
     <t>2019-06-22</t>
   </si>
   <si>
-    <t>2020-01-01</t>
+    <t>2020-06-21</t>
+  </si>
+  <si>
+    <t>2020-06-22</t>
+  </si>
+  <si>
+    <t>2020-08-01</t>
   </si>
   <si>
     <t>Beta</t>
@@ -93,6 +105,12 @@
   </si>
   <si>
     <t>FI</t>
+  </si>
+  <si>
+    <t>2018-11-06</t>
+  </si>
+  <si>
+    <t>2018-11-07</t>
   </si>
   <si>
     <t>2019-11-06</t>
@@ -508,18 +526,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -583,19 +601,19 @@
         <v>16</v>
       </c>
       <c r="H2">
+        <v>930</v>
+      </c>
+      <c r="I2">
         <v>124</v>
       </c>
-      <c r="I2">
-        <v>930</v>
-      </c>
       <c r="J2">
-        <v>60.91</v>
+        <v>59.24</v>
       </c>
       <c r="K2">
-        <v>119228</v>
+        <v>115962</v>
       </c>
       <c r="L2">
-        <v>56644.72</v>
+        <v>55093.06</v>
       </c>
     </row>
     <row r="3">
@@ -627,10 +645,10 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>61.03</v>
+        <v>59.71</v>
       </c>
       <c r="K3">
-        <v>119466</v>
+        <v>116890</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -659,223 +677,223 @@
         <v>18</v>
       </c>
       <c r="H4">
-        <v>138</v>
+        <v>1957.5</v>
       </c>
       <c r="I4">
-        <v>1035</v>
+        <v>261</v>
       </c>
       <c r="J4">
-        <v>62.25</v>
+        <v>60.91</v>
       </c>
       <c r="K4">
-        <v>121855</v>
+        <v>119228</v>
       </c>
       <c r="L4">
-        <v>64429.08</v>
+        <v>119228</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
       </c>
       <c r="G5" t="s">
         <v>18</v>
       </c>
       <c r="H5">
-        <v>262</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>1965</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>46.87</v>
+        <v>61.03</v>
       </c>
       <c r="K5">
-        <v>91740</v>
+        <v>119466</v>
       </c>
       <c r="L5">
-        <v>92091.49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H6">
-        <v>262</v>
+        <v>1950</v>
       </c>
       <c r="I6">
-        <v>1965</v>
+        <v>260</v>
       </c>
       <c r="J6">
-        <v>42.8</v>
+        <v>62.25</v>
       </c>
       <c r="K6">
-        <v>83785</v>
+        <v>121855</v>
       </c>
       <c r="L6">
-        <v>84106.02</v>
+        <v>121388.12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E7">
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H7">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="I7">
-        <v>1665</v>
+        <v>30</v>
       </c>
       <c r="J7">
-        <v>41.2</v>
+        <v>63.18</v>
       </c>
       <c r="K7">
-        <v>80655</v>
+        <v>123683</v>
       </c>
       <c r="L7">
-        <v>68603.1</v>
+        <v>14216.44</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
       <c r="D8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>5062.5</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>675</v>
       </c>
       <c r="J8">
-        <v>41.29</v>
+        <v>46.87</v>
       </c>
       <c r="K8">
-        <v>80816</v>
+        <v>91740</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>237258.62</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E9">
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H9">
-        <v>40</v>
+        <v>5062.5</v>
       </c>
       <c r="I9">
-        <v>300</v>
+        <v>675</v>
       </c>
       <c r="J9">
-        <v>42.11</v>
+        <v>42.8</v>
       </c>
       <c r="K9">
-        <v>82432</v>
+        <v>83785</v>
       </c>
       <c r="L9">
-        <v>12633.26</v>
+        <v>216685.34</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>31</v>
       </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -884,57 +902,57 @@
         <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="H10">
-        <v>262</v>
+        <v>1665</v>
       </c>
       <c r="I10">
-        <v>1965</v>
+        <v>222</v>
       </c>
       <c r="J10">
-        <v>29.45</v>
+        <v>40.07</v>
       </c>
       <c r="K10">
-        <v>57643</v>
+        <v>78446</v>
       </c>
       <c r="L10">
-        <v>57863.85</v>
+        <v>66724.18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
         <v>33</v>
       </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>4</v>
-      </c>
-      <c r="F11" t="s">
-        <v>15</v>
-      </c>
       <c r="G11" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="H11">
-        <v>262</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>1965</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>40.4</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>79074</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -942,192 +960,496 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G12" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="H12">
-        <v>262</v>
+        <v>1957.5</v>
       </c>
       <c r="I12">
-        <v>1965</v>
+        <v>261</v>
       </c>
       <c r="J12">
-        <v>28.85</v>
+        <v>41.2</v>
       </c>
       <c r="K12">
-        <v>56471</v>
+        <v>80655</v>
       </c>
       <c r="L12">
-        <v>56687.36</v>
+        <v>80655</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13">
         <v>4</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="G13" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="H13">
-        <v>262</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>1965</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>46.87</v>
+        <v>41.29</v>
       </c>
       <c r="K13">
-        <v>91740</v>
+        <v>80816</v>
       </c>
       <c r="L13">
-        <v>92091.49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14">
         <v>4</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H14">
-        <v>124</v>
+        <v>1440</v>
       </c>
       <c r="I14">
-        <v>930</v>
+        <v>192</v>
       </c>
       <c r="J14">
-        <v>36.44</v>
+        <v>42.11</v>
       </c>
       <c r="K14">
-        <v>71329</v>
+        <v>82432</v>
       </c>
       <c r="L14">
-        <v>33888.11</v>
+        <v>60639.63</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G15" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>5062.5</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>675</v>
       </c>
       <c r="J15">
-        <v>36.51</v>
+        <v>29.45</v>
       </c>
       <c r="K15">
-        <v>71472</v>
+        <v>57643</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>149076.72</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
         <v>41</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16">
+        <v>5062.5</v>
+      </c>
+      <c r="I16">
+        <v>675</v>
+      </c>
+      <c r="J16">
+        <v>37.12</v>
+      </c>
+      <c r="K16">
+        <v>72660</v>
+      </c>
+      <c r="L16">
+        <v>187913.79</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
         <v>42</v>
       </c>
-      <c r="C16" t="s">
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17">
+        <v>5062.5</v>
+      </c>
+      <c r="I17">
+        <v>675</v>
+      </c>
+      <c r="J17">
+        <v>28.85</v>
+      </c>
+      <c r="K17">
+        <v>56471</v>
+      </c>
+      <c r="L17">
+        <v>146045.69</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18">
+        <v>5062.5</v>
+      </c>
+      <c r="I18">
+        <v>675</v>
+      </c>
+      <c r="J18">
+        <v>46.87</v>
+      </c>
+      <c r="K18">
+        <v>91740</v>
+      </c>
+      <c r="L18">
+        <v>237258.62</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
         <v>14</v>
       </c>
-      <c r="D16">
+      <c r="D19">
         <v>3</v>
       </c>
-      <c r="E16">
-        <v>4</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19">
+        <v>930</v>
+      </c>
+      <c r="I19">
+        <v>124</v>
+      </c>
+      <c r="J19">
+        <v>35.44</v>
+      </c>
+      <c r="K19">
+        <v>69375</v>
+      </c>
+      <c r="L19">
+        <v>32959.77</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
         <v>17</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>35.72</v>
+      </c>
+      <c r="K20">
+        <v>69930</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" t="s">
         <v>18</v>
       </c>
-      <c r="H16">
-        <v>138</v>
-      </c>
-      <c r="I16">
-        <v>1035</v>
-      </c>
-      <c r="J16">
+      <c r="H21">
+        <v>1957.5</v>
+      </c>
+      <c r="I21">
+        <v>261</v>
+      </c>
+      <c r="J21">
+        <v>36.44</v>
+      </c>
+      <c r="K21">
+        <v>71329</v>
+      </c>
+      <c r="L21">
+        <v>71329</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>36.51</v>
+      </c>
+      <c r="K22">
+        <v>71472</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23">
+        <v>1950</v>
+      </c>
+      <c r="I23">
+        <v>260</v>
+      </c>
+      <c r="J23">
         <v>37.24</v>
       </c>
-      <c r="K16">
+      <c r="K23">
         <v>72901</v>
       </c>
-      <c r="L16">
-        <v>38545.36</v>
+      <c r="L23">
+        <v>72621.69</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24">
+        <v>225</v>
+      </c>
+      <c r="I24">
+        <v>30</v>
+      </c>
+      <c r="J24">
+        <v>37.8</v>
+      </c>
+      <c r="K24">
+        <v>73995</v>
+      </c>
+      <c r="L24">
+        <v>8505.17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>